<commit_message>
Update CDM-5 and DRP
Atualizado o CDM-5 com o preenchimento das observações na Sessão 2,
anteriormente esquecidas, e atualização do DRP conforme previsto no
CDM-5.
</commit_message>
<xml_diff>
--- a/Projeto/GPR/PG2016-1-CDM-5.xlsx
+++ b/Projeto/GPR/PG2016-1-CDM-5.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>1. Acompanhamento de Execução</t>
   </si>
@@ -110,6 +110,20 @@
   </si>
   <si>
     <t>AT23/AT26</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Observações: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Devido a fase final do projeto estar sendo realizada sem maiores problemas relacionados à complexidade, o risco que trata desse assunto será removido do DRP.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -696,7 +710,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I12"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -949,7 +963,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>

</xml_diff>